<commit_message>
Further work on write_or_append_to_excel function in models notebook to generalize it for multiple table types
</commit_message>
<xml_diff>
--- a/data/visualizations_public.xlsx
+++ b/data/visualizations_public.xlsx
@@ -2,28 +2,45 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="36500" yWindow="-6220" windowWidth="29400" windowHeight="17260" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Desc1 CB, week_fyear 172" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="14"/>
     </font>
     <font>
       <b val="1"/>
@@ -55,7 +72,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -64,6 +81,112 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -93,18 +216,10 @@
     <border>
       <left style="thin"/>
       <right style="thin"/>
-      <top style="thick">
+      <top style="thin"/>
+      <bottom style="thick">
         <color rgb="00000000"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
+      </bottom>
     </border>
     <border>
       <left style="thin"/>
@@ -119,22 +234,8 @@
       <right style="thick">
         <color rgb="00000000"/>
       </right>
-      <top style="thick">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
+      <top style="thin"/>
+      <bottom style="thick">
         <color rgb="00000000"/>
       </bottom>
     </border>
@@ -154,41 +255,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -559,267 +676,267 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" style="9" min="3" max="3"/>
+    <col width="12" customWidth="1" style="9" min="4" max="4"/>
+    <col width="12" customWidth="1" style="9" min="5" max="5"/>
+    <col width="12" customWidth="1" style="9" min="6" max="6"/>
+    <col width="12" customWidth="1" style="9" min="7" max="7"/>
+    <col width="12" customWidth="1" style="9" min="8" max="8"/>
+    <col width="12" customWidth="1" style="9" min="9" max="9"/>
+    <col width="12" customWidth="1" style="9" min="10" max="10"/>
+    <col width="12" customWidth="1" style="9" min="11" max="11"/>
+    <col width="12" customWidth="1" style="9" min="12" max="12"/>
+    <col width="12" customWidth="1" style="9" min="13" max="13"/>
   </cols>
   <sheetData>
-    <row r="1" ht="50" customHeight="1">
-      <c r="B1" s="1" t="inlineStr">
+    <row r="1" ht="50" customHeight="1" s="9">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Desc1 CB Comparison Table for Periods 4 and 5</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1">
-      <c r="B2" s="4" t="inlineStr"/>
-      <c r="C2" s="3" t="inlineStr">
+    <row r="2" ht="25" customHeight="1" s="9">
+      <c r="B2" s="11" t="inlineStr"/>
+      <c r="C2" s="12" t="inlineStr">
         <is>
           <t>Acct 1</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="D2" s="12" t="n"/>
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>Acct 10</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="12" t="inlineStr">
         <is>
           <t>Acct 11</t>
         </is>
       </c>
-      <c r="G2" s="3" t="n"/>
-      <c r="H2" s="3" t="inlineStr">
+      <c r="G2" s="12" t="n"/>
+      <c r="H2" s="12" t="inlineStr">
         <is>
           <t>Acct 4</t>
         </is>
       </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="inlineStr">
+      <c r="I2" s="12" t="n"/>
+      <c r="J2" s="12" t="inlineStr">
         <is>
           <t>Acct 5</t>
         </is>
       </c>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="3" t="inlineStr">
+      <c r="K2" s="12" t="n"/>
+      <c r="L2" s="12" t="inlineStr">
         <is>
           <t>Trends</t>
         </is>
       </c>
-      <c r="M2" s="3" t="n"/>
+      <c r="M2" s="12" t="n"/>
     </row>
-    <row r="3" ht="25" customHeight="1">
-      <c r="B3" s="4" t="inlineStr">
+    <row r="3" ht="25" customHeight="1" s="9">
+      <c r="B3" s="13" t="inlineStr">
         <is>
           <t>Period</t>
         </is>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="L3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="M3" s="14" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1">
-      <c r="B4" s="9" t="n">
+    <row r="4" ht="25" customHeight="1" s="9">
+      <c r="B4" s="15" t="n">
         <v>2020</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="16" t="n">
         <v>0.03</v>
       </c>
-      <c r="D4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="n">
+      <c r="D4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16" t="n">
         <v>0.93</v>
       </c>
-      <c r="F4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="n">
+      <c r="F4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16" t="n">
         <v>0.1</v>
       </c>
-      <c r="I4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="n">
+      <c r="I4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="16" t="n">
         <v>0.73</v>
       </c>
-      <c r="K4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6" t="inlineStr">
+      <c r="K4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="16" t="inlineStr">
         <is>
           <t>downward</t>
         </is>
       </c>
-      <c r="M4" s="6" t="inlineStr">
+      <c r="M4" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve"> -- </t>
         </is>
       </c>
     </row>
-    <row r="5" ht="25" customHeight="1">
-      <c r="B5" s="4" t="n">
+    <row r="5" ht="25" customHeight="1" s="9">
+      <c r="B5" s="15" t="n">
         <v>2021</v>
       </c>
-      <c r="C5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7" t="n">
+      <c r="C5" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16" t="n">
         <v>0.13</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="16" t="n">
         <v>0.11</v>
       </c>
-      <c r="G5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7" t="n">
+      <c r="G5" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16" t="n">
         <v>0.8</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="16" t="n">
         <v>0.72</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="J5" s="16" t="n">
         <v>0.93</v>
       </c>
-      <c r="K5" s="7" t="n">
+      <c r="K5" s="16" t="n">
         <v>0.93</v>
       </c>
-      <c r="L5" s="7" t="inlineStr">
+      <c r="L5" s="16" t="inlineStr">
         <is>
           <t>upward</t>
         </is>
       </c>
-      <c r="M5" s="7" t="inlineStr">
+      <c r="M5" s="16" t="inlineStr">
         <is>
           <t>peaks</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="25" customHeight="1">
-      <c r="B6" s="4" t="n">
+    <row r="6" ht="25" customHeight="1" s="9">
+      <c r="B6" s="15" t="n">
         <v>2022</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="16" t="n">
         <v>0.52</v>
       </c>
-      <c r="D6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="n">
+      <c r="D6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16" t="n">
         <v>0.37</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="16" t="n">
         <v>0.63</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="16" t="n">
         <v>0.15</v>
       </c>
-      <c r="J6" s="7" t="n">
+      <c r="J6" s="16" t="n">
         <v>0.98</v>
       </c>
-      <c r="K6" s="7" t="n">
+      <c r="K6" s="16" t="n">
         <v>0.64</v>
       </c>
-      <c r="L6" s="7" t="inlineStr">
+      <c r="L6" s="16" t="inlineStr">
         <is>
           <t>peaks</t>
         </is>
       </c>
-      <c r="M6" s="7" t="inlineStr">
+      <c r="M6" s="16" t="inlineStr">
         <is>
           <t>troughs</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="25" customHeight="1">
-      <c r="B7" s="4" t="n">
+    <row r="7" ht="25" customHeight="1" s="9">
+      <c r="B7" s="15" t="n">
         <v>2023</v>
       </c>
-      <c r="C7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="n">
+      <c r="C7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16" t="n">
         <v>0.98</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="H7" s="16" t="n">
         <v>0.45</v>
       </c>
-      <c r="I7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7" t="n">
+      <c r="I7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16" t="n">
         <v>0.73</v>
       </c>
-      <c r="K7" s="7" t="n">
+      <c r="K7" s="16" t="n">
         <v>0.06</v>
       </c>
-      <c r="L7" s="7" t="inlineStr">
+      <c r="L7" s="16" t="inlineStr">
         <is>
           <t>downward</t>
         </is>
       </c>
-      <c r="M7" s="7" t="inlineStr">
+      <c r="M7" s="16" t="inlineStr">
         <is>
           <t>troughs</t>
         </is>

</xml_diff>

<commit_message>
Finished work on Granger Causality Visualizations and write_or_append_to_excel function
</commit_message>
<xml_diff>
--- a/data/visualizations_public.xlsx
+++ b/data/visualizations_public.xlsx
@@ -2,45 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="36500" yWindow="-6220" windowWidth="29400" windowHeight="17260" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Desc1 CB, week_fyear 172" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="lag_stats_CB_172" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="lag_stats_summary_P5_FY23" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="20"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="14"/>
     </font>
     <font>
       <b val="1"/>
@@ -72,118 +56,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -251,61 +129,81 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -668,7 +566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="B1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,267 +574,263 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" style="9" min="3" max="3"/>
-    <col width="12" customWidth="1" style="9" min="4" max="4"/>
-    <col width="12" customWidth="1" style="9" min="5" max="5"/>
-    <col width="12" customWidth="1" style="9" min="6" max="6"/>
-    <col width="12" customWidth="1" style="9" min="7" max="7"/>
-    <col width="12" customWidth="1" style="9" min="8" max="8"/>
-    <col width="12" customWidth="1" style="9" min="9" max="9"/>
-    <col width="12" customWidth="1" style="9" min="10" max="10"/>
-    <col width="12" customWidth="1" style="9" min="11" max="11"/>
-    <col width="12" customWidth="1" style="9" min="12" max="12"/>
-    <col width="12" customWidth="1" style="9" min="13" max="13"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="11" max="11"/>
+    <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
-    <row r="1" ht="50" customHeight="1" s="9">
-      <c r="B1" s="10" t="inlineStr">
+    <row r="1" ht="50" customHeight="1">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Desc1 CB Comparison Table for Periods 4 and 5</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1" s="9">
-      <c r="B2" s="11" t="inlineStr"/>
-      <c r="C2" s="12" t="inlineStr">
+    <row r="2" ht="25" customHeight="1">
+      <c r="B2" s="2" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Acct 1</t>
         </is>
       </c>
-      <c r="D2" s="12" t="n"/>
-      <c r="E2" s="12" t="inlineStr">
+      <c r="D2" s="8" t="n"/>
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Acct 10</t>
         </is>
       </c>
-      <c r="F2" s="12" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Acct 11</t>
         </is>
       </c>
-      <c r="G2" s="12" t="n"/>
-      <c r="H2" s="12" t="inlineStr">
+      <c r="G2" s="8" t="n"/>
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>Acct 4</t>
         </is>
       </c>
-      <c r="I2" s="12" t="n"/>
-      <c r="J2" s="12" t="inlineStr">
+      <c r="I2" s="8" t="n"/>
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t>Acct 5</t>
         </is>
       </c>
-      <c r="K2" s="12" t="n"/>
-      <c r="L2" s="12" t="inlineStr">
+      <c r="K2" s="8" t="n"/>
+      <c r="L2" s="3" t="inlineStr">
         <is>
           <t>Trends</t>
         </is>
       </c>
-      <c r="M2" s="12" t="n"/>
-    </row>
-    <row r="3" ht="25" customHeight="1" s="9">
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t>Period</t>
-        </is>
-      </c>
-      <c r="C3" s="14" t="n">
+      <c r="M2" s="8" t="n"/>
+    </row>
+    <row r="3" ht="25" customHeight="1">
+      <c r="B3" s="4" t="inlineStr"/>
+      <c r="C3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="14" t="n">
+      <c r="E3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="G3" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="14" t="n">
+      <c r="H3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="14" t="n">
+      <c r="I3" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="J3" s="14" t="n">
+      <c r="J3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="K3" s="14" t="n">
+      <c r="K3" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="L3" s="14" t="n">
+      <c r="L3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="M3" s="14" t="n">
+      <c r="M3" s="5" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" s="9">
-      <c r="B4" s="15" t="n">
+    <row r="4" ht="25" customHeight="1">
+      <c r="B4" s="6" t="n">
         <v>2020</v>
       </c>
-      <c r="C4" s="16" t="n">
+      <c r="C4" s="7" t="n">
         <v>0.03</v>
       </c>
-      <c r="D4" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="16" t="n">
+      <c r="D4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="n">
         <v>0.93</v>
       </c>
-      <c r="F4" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="16" t="n">
+      <c r="F4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="I4" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="16" t="n">
+      <c r="I4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7" t="n">
         <v>0.73</v>
       </c>
-      <c r="K4" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="16" t="inlineStr">
+      <c r="K4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12" t="inlineStr">
         <is>
           <t>downward</t>
         </is>
       </c>
-      <c r="M4" s="16" t="inlineStr">
+      <c r="M4" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve"> -- </t>
         </is>
       </c>
     </row>
-    <row r="5" ht="25" customHeight="1" s="9">
-      <c r="B5" s="15" t="n">
+    <row r="5" ht="25" customHeight="1">
+      <c r="B5" s="6" t="n">
         <v>2021</v>
       </c>
-      <c r="C5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="16" t="n">
+      <c r="C5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="n">
         <v>0.13</v>
       </c>
-      <c r="F5" s="16" t="n">
+      <c r="F5" s="7" t="n">
         <v>0.11</v>
       </c>
-      <c r="G5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16" t="n">
+      <c r="G5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7" t="n">
         <v>0.8</v>
       </c>
-      <c r="I5" s="16" t="n">
+      <c r="I5" s="7" t="n">
         <v>0.72</v>
       </c>
-      <c r="J5" s="16" t="n">
+      <c r="J5" s="7" t="n">
         <v>0.93</v>
       </c>
-      <c r="K5" s="16" t="n">
+      <c r="K5" s="7" t="n">
         <v>0.93</v>
       </c>
-      <c r="L5" s="16" t="inlineStr">
+      <c r="L5" s="12" t="inlineStr">
         <is>
           <t>upward</t>
         </is>
       </c>
-      <c r="M5" s="16" t="inlineStr">
+      <c r="M5" s="12" t="inlineStr">
         <is>
           <t>peaks</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="25" customHeight="1" s="9">
-      <c r="B6" s="15" t="n">
+    <row r="6" ht="25" customHeight="1">
+      <c r="B6" s="6" t="n">
         <v>2022</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="7" t="n">
         <v>0.52</v>
       </c>
-      <c r="D6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="16" t="n">
+      <c r="D6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="n">
         <v>0.37</v>
       </c>
-      <c r="H6" s="16" t="n">
+      <c r="H6" s="7" t="n">
         <v>0.63</v>
       </c>
-      <c r="I6" s="16" t="n">
+      <c r="I6" s="7" t="n">
         <v>0.15</v>
       </c>
-      <c r="J6" s="16" t="n">
+      <c r="J6" s="7" t="n">
         <v>0.98</v>
       </c>
-      <c r="K6" s="16" t="n">
+      <c r="K6" s="7" t="n">
         <v>0.64</v>
       </c>
-      <c r="L6" s="16" t="inlineStr">
+      <c r="L6" s="12" t="inlineStr">
         <is>
           <t>peaks</t>
         </is>
       </c>
-      <c r="M6" s="16" t="inlineStr">
+      <c r="M6" s="12" t="inlineStr">
         <is>
           <t>troughs</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="25" customHeight="1" s="9">
-      <c r="B7" s="15" t="n">
+    <row r="7" ht="25" customHeight="1">
+      <c r="B7" s="6" t="n">
         <v>2023</v>
       </c>
-      <c r="C7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="16" t="n">
+      <c r="C7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="n">
         <v>0.98</v>
       </c>
-      <c r="H7" s="16" t="n">
+      <c r="H7" s="7" t="n">
         <v>0.45</v>
       </c>
-      <c r="I7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="16" t="n">
+      <c r="I7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7" t="n">
         <v>0.73</v>
       </c>
-      <c r="K7" s="16" t="n">
+      <c r="K7" s="7" t="n">
         <v>0.06</v>
       </c>
-      <c r="L7" s="16" t="inlineStr">
+      <c r="L7" s="12" t="inlineStr">
         <is>
           <t>downward</t>
         </is>
       </c>
-      <c r="M7" s="16" t="inlineStr">
+      <c r="M7" s="12" t="inlineStr">
         <is>
           <t>troughs</t>
         </is>
@@ -953,4 +847,161 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Desc1 Lag Table for Period 5 and FY23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="25" customHeight="1">
+      <c r="B2" s="9" t="n"/>
+      <c r="C2" s="10" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>Week FY</t>
+        </is>
+      </c>
+      <c r="F2" s="10" t="inlineStr">
+        <is>
+          <t>Lag</t>
+        </is>
+      </c>
+      <c r="G2" s="10" t="inlineStr">
+        <is>
+          <t>Period</t>
+        </is>
+      </c>
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>FY</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1">
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>187871.26</v>
+      </c>
+      <c r="E3" s="12" t="n">
+        <v>172</v>
+      </c>
+      <c r="F3" s="12" t="inlineStr">
+        <is>
+          <t>[3, 5]</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="12" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1">
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>freq</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0.08076165462902167</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>173</v>
+      </c>
+      <c r="F4" s="12" t="inlineStr">
+        <is>
+          <t>[3, 5]</t>
+        </is>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" s="12" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1">
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>EI</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>27046.9</v>
+      </c>
+      <c r="E5" s="12" t="n">
+        <v>171</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>[5]</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" s="12" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Continued work on presentation and cleanup
</commit_message>
<xml_diff>
--- a/data/visualizations_public.xlsx
+++ b/data/visualizations_public.xlsx
@@ -2,29 +2,90 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="36800" yWindow="-7680" windowWidth="29400" windowHeight="17260" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="lag_stats_CB_172" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="lag_stats_summary_P5_FY23" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Time Series Pivot Table" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sample Transformed Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Unique Counts" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Date Range" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Two Sample Ttest Desc1s" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="14"/>
     </font>
     <font>
       <b val="1"/>
@@ -56,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -65,6 +126,231 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -73,23 +359,10 @@
     <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin"/>
@@ -100,22 +373,22 @@
       </bottom>
     </border>
     <border>
+      <left/>
+      <right style="thick">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thick">
         <color rgb="00000000"/>
       </right>
       <top style="thin"/>
       <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thick">
-        <color rgb="00000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -129,81 +402,113 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -572,265 +877,255 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
-    <col width="14" customWidth="1" min="10" max="10"/>
-    <col width="14" customWidth="1" min="11" max="11"/>
-    <col width="14" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
+    <col width="14" customWidth="1" style="24" min="3" max="13"/>
   </cols>
   <sheetData>
-    <row r="1" ht="50" customHeight="1">
-      <c r="B1" s="1" t="inlineStr">
+    <row r="1" ht="50" customHeight="1" s="24">
+      <c r="B1" s="23" t="inlineStr">
         <is>
           <t>Desc1 CB Comparison Table for Periods 4 and 5</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1">
-      <c r="B2" s="2" t="inlineStr"/>
-      <c r="C2" s="3" t="inlineStr">
+    <row r="2" ht="25" customHeight="1" s="24">
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="21" t="inlineStr">
         <is>
           <t>Acct 1</t>
         </is>
       </c>
-      <c r="D2" s="8" t="n"/>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="D2" s="22" t="n"/>
+      <c r="E2" s="21" t="inlineStr">
         <is>
           <t>Acct 10</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="21" t="inlineStr">
         <is>
           <t>Acct 11</t>
         </is>
       </c>
-      <c r="G2" s="8" t="n"/>
-      <c r="H2" s="3" t="inlineStr">
+      <c r="G2" s="22" t="n"/>
+      <c r="H2" s="21" t="inlineStr">
         <is>
           <t>Acct 4</t>
         </is>
       </c>
-      <c r="I2" s="8" t="n"/>
-      <c r="J2" s="3" t="inlineStr">
+      <c r="I2" s="22" t="n"/>
+      <c r="J2" s="21" t="inlineStr">
         <is>
           <t>Acct 5</t>
         </is>
       </c>
-      <c r="K2" s="8" t="n"/>
-      <c r="L2" s="3" t="inlineStr">
+      <c r="K2" s="22" t="n"/>
+      <c r="L2" s="21" t="inlineStr">
         <is>
           <t>Trends</t>
         </is>
       </c>
-      <c r="M2" s="8" t="n"/>
-    </row>
-    <row r="3" ht="25" customHeight="1">
-      <c r="B3" s="4" t="inlineStr"/>
-      <c r="C3" s="5" t="n">
+      <c r="M2" s="22" t="n"/>
+    </row>
+    <row r="3" ht="25" customHeight="1" s="24">
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="4" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1">
-      <c r="B4" s="6" t="n">
+    <row r="4" ht="25" customHeight="1" s="24">
+      <c r="B4" s="5" t="n">
         <v>2020</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>0.03</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>0.93</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="G4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="6" t="n">
         <v>0.1</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="7" t="n">
+      <c r="J4" s="6" t="n">
         <v>0.73</v>
       </c>
-      <c r="K4" s="7" t="n">
+      <c r="K4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="12" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>downward</t>
         </is>
       </c>
-      <c r="M4" s="12" t="inlineStr">
+      <c r="M4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve"> -- </t>
         </is>
       </c>
     </row>
-    <row r="5" ht="25" customHeight="1">
-      <c r="B5" s="6" t="n">
+    <row r="5" ht="25" customHeight="1" s="24">
+      <c r="B5" s="5" t="n">
         <v>2021</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>0.13</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>0.11</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="6" t="n">
         <v>0.8</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="6" t="n">
         <v>0.72</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="J5" s="6" t="n">
         <v>0.93</v>
       </c>
-      <c r="K5" s="7" t="n">
+      <c r="K5" s="6" t="n">
         <v>0.93</v>
       </c>
-      <c r="L5" s="12" t="inlineStr">
+      <c r="L5" s="9" t="inlineStr">
         <is>
           <t>upward</t>
         </is>
       </c>
-      <c r="M5" s="12" t="inlineStr">
+      <c r="M5" s="9" t="inlineStr">
         <is>
           <t>peaks</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="25" customHeight="1">
-      <c r="B6" s="6" t="n">
+    <row r="6" ht="25" customHeight="1" s="24">
+      <c r="B6" s="5" t="n">
         <v>2022</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>0.52</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="6" t="n">
         <v>0.37</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="6" t="n">
         <v>0.63</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="6" t="n">
         <v>0.15</v>
       </c>
-      <c r="J6" s="7" t="n">
+      <c r="J6" s="6" t="n">
         <v>0.98</v>
       </c>
-      <c r="K6" s="7" t="n">
+      <c r="K6" s="6" t="n">
         <v>0.64</v>
       </c>
-      <c r="L6" s="12" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>peaks</t>
         </is>
       </c>
-      <c r="M6" s="12" t="inlineStr">
+      <c r="M6" s="9" t="inlineStr">
         <is>
           <t>troughs</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="25" customHeight="1">
-      <c r="B7" s="6" t="n">
+    <row r="7" ht="25" customHeight="1" s="24">
+      <c r="B7" s="5" t="n">
         <v>2023</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="6" t="n">
         <v>0.98</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="H7" s="6" t="n">
         <v>0.45</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="7" t="n">
+      <c r="J7" s="6" t="n">
         <v>0.73</v>
       </c>
-      <c r="K7" s="7" t="n">
+      <c r="K7" s="6" t="n">
         <v>0.06</v>
       </c>
-      <c r="L7" s="12" t="inlineStr">
+      <c r="L7" s="9" t="inlineStr">
         <is>
           <t>downward</t>
         </is>
       </c>
-      <c r="M7" s="12" t="inlineStr">
+      <c r="M7" s="9" t="inlineStr">
         <is>
           <t>troughs</t>
         </is>
@@ -861,140 +1156,135 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" style="24" min="3" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="50" customHeight="1">
-      <c r="B1" s="1" t="inlineStr">
+    <row r="1" ht="50" customHeight="1" s="24">
+      <c r="B1" s="23" t="inlineStr">
         <is>
           <t>Desc1 Lag Table for Period 5 and FY23</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1">
-      <c r="B2" s="9" t="n"/>
-      <c r="C2" s="10" t="inlineStr">
+    <row r="2" ht="25" customHeight="1" s="24">
+      <c r="B2" s="7" t="n"/>
+      <c r="C2" s="8" t="inlineStr">
         <is>
           <t>Metric</t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D2" s="8" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>Week FY</t>
         </is>
       </c>
-      <c r="F2" s="10" t="inlineStr">
+      <c r="F2" s="8" t="inlineStr">
         <is>
           <t>Lag</t>
         </is>
       </c>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="G2" s="8" t="inlineStr">
         <is>
           <t>Period</t>
         </is>
       </c>
-      <c r="H2" s="10" t="inlineStr">
+      <c r="H2" s="8" t="inlineStr">
         <is>
           <t>FY</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="25" customHeight="1">
-      <c r="B3" s="6" t="inlineStr">
+    <row r="3" ht="25" customHeight="1" s="24">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>CB</t>
         </is>
       </c>
-      <c r="C3" s="12" t="inlineStr">
+      <c r="C3" s="9" t="inlineStr">
         <is>
           <t>sum</t>
         </is>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>187871.26</v>
       </c>
-      <c r="E3" s="12" t="n">
+      <c r="E3" s="9" t="n">
         <v>172</v>
       </c>
-      <c r="F3" s="12" t="inlineStr">
+      <c r="F3" s="9" t="inlineStr">
         <is>
           <t>[3, 5]</t>
         </is>
       </c>
-      <c r="G3" s="12" t="n">
+      <c r="G3" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="H3" s="12" t="n">
+      <c r="H3" s="9" t="n">
         <v>2023</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1">
-      <c r="B4" s="6" t="inlineStr">
+    <row r="4" ht="25" customHeight="1" s="24">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>FJ</t>
         </is>
       </c>
-      <c r="C4" s="12" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
           <t>freq</t>
         </is>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>0.08076165462902167</v>
       </c>
-      <c r="E4" s="12" t="n">
+      <c r="E4" s="9" t="n">
         <v>173</v>
       </c>
-      <c r="F4" s="12" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>[3, 5]</t>
         </is>
       </c>
-      <c r="G4" s="12" t="n">
+      <c r="G4" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="H4" s="12" t="n">
+      <c r="H4" s="9" t="n">
         <v>2023</v>
       </c>
     </row>
-    <row r="5" ht="25" customHeight="1">
-      <c r="B5" s="6" t="inlineStr">
+    <row r="5" ht="25" customHeight="1" s="24">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>EI</t>
         </is>
       </c>
-      <c r="C5" s="12" t="inlineStr">
+      <c r="C5" s="9" t="inlineStr">
         <is>
           <t>mean</t>
         </is>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>27046.9</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="9" t="n">
         <v>171</v>
       </c>
-      <c r="F5" s="12" t="inlineStr">
+      <c r="F5" s="9" t="inlineStr">
         <is>
           <t>[5]</t>
         </is>
       </c>
-      <c r="G5" s="12" t="n">
+      <c r="G5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="H5" s="12" t="n">
+      <c r="H5" s="9" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -1004,4 +1294,967 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" style="24" min="3" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1" s="24">
+      <c r="B1" s="23" t="inlineStr">
+        <is>
+          <t>Desc1 Transactions by First 5 Time Periods</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="25" customHeight="1" s="24">
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>Desc1</t>
+        </is>
+      </c>
+      <c r="C2" s="8" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="D2" s="8" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="E2" s="8" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="F2" s="8" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="G2" s="8" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" s="24">
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>-32.93</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G3" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" s="24">
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>1797.68</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>1989.7</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>2055.58</t>
+        </is>
+      </c>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>-41.11</t>
+        </is>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
+          <t>4749.57</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" s="24">
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t>10803.99</t>
+        </is>
+      </c>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t>9977.31</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="inlineStr">
+        <is>
+          <t>10639.95</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>6342.93</t>
+        </is>
+      </c>
+      <c r="G5" s="9" t="inlineStr">
+        <is>
+          <t>6875.81</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" s="24">
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t>188698.66</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>216077.87</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t>126605.53</t>
+        </is>
+      </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>86274.34</t>
+        </is>
+      </c>
+      <c r="G6" s="9" t="inlineStr">
+        <is>
+          <t>206333.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" s="24">
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>AE</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t>28903.77</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>31044.42</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
+        <is>
+          <t>29362.89</t>
+        </is>
+      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>16930.15</t>
+        </is>
+      </c>
+      <c r="G7" s="9" t="inlineStr">
+        <is>
+          <t>10065.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" s="24">
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>AF</t>
+        </is>
+      </c>
+      <c r="C8" s="9" t="inlineStr">
+        <is>
+          <t>10566.12</t>
+        </is>
+      </c>
+      <c r="D8" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>3012.25</t>
+        </is>
+      </c>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>2761.65</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="25" customHeight="1" s="24">
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>AG</t>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t>409.55</t>
+        </is>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>335.92</t>
+        </is>
+      </c>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F9" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G9" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="25" customHeight="1" s="24">
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="C10" s="9" t="inlineStr">
+        <is>
+          <t>1115.95</t>
+        </is>
+      </c>
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t>1428.91</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="inlineStr">
+        <is>
+          <t>45.77</t>
+        </is>
+      </c>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>1233.47</t>
+        </is>
+      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>565.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="25" customHeight="1" s="24">
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="C11" s="9" t="inlineStr">
+        <is>
+          <t>114.49</t>
+        </is>
+      </c>
+      <c r="D11" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F11" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="25" customHeight="1" s="24">
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>AJ</t>
+        </is>
+      </c>
+      <c r="C12" s="9" t="inlineStr">
+        <is>
+          <t>32731.02</t>
+        </is>
+      </c>
+      <c r="D12" s="9" t="inlineStr">
+        <is>
+          <t>5660.36</t>
+        </is>
+      </c>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>10043.76</t>
+        </is>
+      </c>
+      <c r="F12" s="9" t="inlineStr">
+        <is>
+          <t>24703.57</t>
+        </is>
+      </c>
+      <c r="G12" s="9" t="inlineStr">
+        <is>
+          <t>26758.49</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:O7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" style="24" min="3" max="3"/>
+    <col width="14" customWidth="1" style="24" min="4" max="4"/>
+    <col width="14" customWidth="1" style="24" min="5" max="5"/>
+    <col width="14" customWidth="1" style="24" min="6" max="6"/>
+    <col width="14" customWidth="1" style="24" min="7" max="7"/>
+    <col width="14" customWidth="1" style="24" min="8" max="8"/>
+    <col width="14" customWidth="1" style="24" min="9" max="9"/>
+    <col width="14" customWidth="1" style="24" min="10" max="10"/>
+    <col width="14" customWidth="1" style="24" min="11" max="11"/>
+    <col width="14" customWidth="1" style="24" min="12" max="12"/>
+    <col width="14" customWidth="1" style="24" min="13" max="13"/>
+    <col width="14" customWidth="1" style="24" min="14" max="14"/>
+    <col width="14" customWidth="1" style="24" min="15" max="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1" s="24">
+      <c r="B1" s="27" t="inlineStr">
+        <is>
+          <t>Sample Transformed Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="25" customHeight="1" s="24">
+      <c r="B2" s="28" t="n"/>
+      <c r="C2" s="29" t="inlineStr">
+        <is>
+          <t>Desc1</t>
+        </is>
+      </c>
+      <c r="D2" s="29" t="inlineStr">
+        <is>
+          <t>Desc2</t>
+        </is>
+      </c>
+      <c r="E2" s="29" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F2" s="29" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="G2" s="29" t="inlineStr">
+        <is>
+          <t>Debit</t>
+        </is>
+      </c>
+      <c r="H2" s="29" t="inlineStr">
+        <is>
+          <t>Credit</t>
+        </is>
+      </c>
+      <c r="I2" s="29" t="inlineStr">
+        <is>
+          <t>Txn_amt</t>
+        </is>
+      </c>
+      <c r="J2" s="29" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="K2" s="29" t="inlineStr">
+        <is>
+          <t>Fyear</t>
+        </is>
+      </c>
+      <c r="L2" s="29" t="inlineStr">
+        <is>
+          <t>Period</t>
+        </is>
+      </c>
+      <c r="M2" s="29" t="inlineStr">
+        <is>
+          <t>Period_fyear</t>
+        </is>
+      </c>
+      <c r="N2" s="29" t="inlineStr">
+        <is>
+          <t>Week</t>
+        </is>
+      </c>
+      <c r="O2" s="29" t="inlineStr">
+        <is>
+          <t>Week_fyear</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" s="24">
+      <c r="B3" s="30" t="n">
+        <v>28727</v>
+      </c>
+      <c r="C3" s="31" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="D3" s="31" t="n">
+        <v>5324</v>
+      </c>
+      <c r="E3" s="31" t="inlineStr">
+        <is>
+          <t>AU 05324</t>
+        </is>
+      </c>
+      <c r="F3" s="31" t="inlineStr">
+        <is>
+          <t>Acct 4</t>
+        </is>
+      </c>
+      <c r="G3" s="32" t="n">
+        <v>-74.91</v>
+      </c>
+      <c r="H3" s="31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I3" s="32" t="n">
+        <v>74.91</v>
+      </c>
+      <c r="J3" s="34" t="n">
+        <v>44354</v>
+      </c>
+      <c r="K3" s="31" t="n">
+        <v>2021</v>
+      </c>
+      <c r="L3" s="31" t="n">
+        <v>9</v>
+      </c>
+      <c r="M3" s="31" t="n">
+        <v>20</v>
+      </c>
+      <c r="N3" s="31" t="n">
+        <v>23</v>
+      </c>
+      <c r="O3" s="31" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" s="24">
+      <c r="B4" s="30" t="n">
+        <v>53577</v>
+      </c>
+      <c r="C4" s="31" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="D4" s="31" t="n">
+        <v>9866</v>
+      </c>
+      <c r="E4" s="31" t="inlineStr">
+        <is>
+          <t>BR 09866</t>
+        </is>
+      </c>
+      <c r="F4" s="31" t="inlineStr">
+        <is>
+          <t>Acct 4</t>
+        </is>
+      </c>
+      <c r="G4" s="32" t="n">
+        <v>-79.62</v>
+      </c>
+      <c r="H4" s="31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I4" s="32" t="n">
+        <v>79.62</v>
+      </c>
+      <c r="J4" s="34" t="n">
+        <v>44729</v>
+      </c>
+      <c r="K4" s="31" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L4" s="31" t="n">
+        <v>9</v>
+      </c>
+      <c r="M4" s="31" t="n">
+        <v>32</v>
+      </c>
+      <c r="N4" s="31" t="n">
+        <v>24</v>
+      </c>
+      <c r="O4" s="31" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" s="24">
+      <c r="B5" s="30" t="n">
+        <v>36992</v>
+      </c>
+      <c r="C5" s="31" t="inlineStr">
+        <is>
+          <t>CV</t>
+        </is>
+      </c>
+      <c r="D5" s="31" t="n">
+        <v>6521</v>
+      </c>
+      <c r="E5" s="31" t="inlineStr">
+        <is>
+          <t>CV 06521</t>
+        </is>
+      </c>
+      <c r="F5" s="31" t="inlineStr">
+        <is>
+          <t>Acct 4</t>
+        </is>
+      </c>
+      <c r="G5" s="32" t="n">
+        <v>-55.55</v>
+      </c>
+      <c r="H5" s="31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I5" s="32" t="n">
+        <v>55.55</v>
+      </c>
+      <c r="J5" s="34" t="n">
+        <v>44460</v>
+      </c>
+      <c r="K5" s="31" t="n">
+        <v>2021</v>
+      </c>
+      <c r="L5" s="31" t="n">
+        <v>12</v>
+      </c>
+      <c r="M5" s="31" t="n">
+        <v>23</v>
+      </c>
+      <c r="N5" s="31" t="n">
+        <v>38</v>
+      </c>
+      <c r="O5" s="31" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" s="24">
+      <c r="B6" s="30" t="n">
+        <v>33942</v>
+      </c>
+      <c r="C6" s="31" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="D6" s="31" t="n">
+        <v>6040</v>
+      </c>
+      <c r="E6" s="31" t="inlineStr">
+        <is>
+          <t>CA 06040</t>
+        </is>
+      </c>
+      <c r="F6" s="31" t="inlineStr">
+        <is>
+          <t>Acct 6</t>
+        </is>
+      </c>
+      <c r="G6" s="32" t="n">
+        <v>-475.62</v>
+      </c>
+      <c r="H6" s="31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I6" s="32" t="n">
+        <v>475.62</v>
+      </c>
+      <c r="J6" s="34" t="n">
+        <v>44417</v>
+      </c>
+      <c r="K6" s="31" t="n">
+        <v>2021</v>
+      </c>
+      <c r="L6" s="31" t="n">
+        <v>11</v>
+      </c>
+      <c r="M6" s="31" t="n">
+        <v>22</v>
+      </c>
+      <c r="N6" s="31" t="n">
+        <v>32</v>
+      </c>
+      <c r="O6" s="31" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" s="24">
+      <c r="B7" s="30" t="n">
+        <v>53920</v>
+      </c>
+      <c r="C7" s="31" t="inlineStr">
+        <is>
+          <t>FS</t>
+        </is>
+      </c>
+      <c r="D7" s="31" t="n">
+        <v>9940</v>
+      </c>
+      <c r="E7" s="31" t="inlineStr">
+        <is>
+          <t>FS 09940</t>
+        </is>
+      </c>
+      <c r="F7" s="31" t="inlineStr">
+        <is>
+          <t>Acct 9</t>
+        </is>
+      </c>
+      <c r="G7" s="32" t="n">
+        <v>-395.67</v>
+      </c>
+      <c r="H7" s="31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I7" s="32" t="n">
+        <v>395.67</v>
+      </c>
+      <c r="J7" s="34" t="n">
+        <v>44740</v>
+      </c>
+      <c r="K7" s="31" t="n">
+        <v>2022</v>
+      </c>
+      <c r="L7" s="31" t="n">
+        <v>9</v>
+      </c>
+      <c r="M7" s="31" t="n">
+        <v>32</v>
+      </c>
+      <c r="N7" s="31" t="n">
+        <v>26</v>
+      </c>
+      <c r="O7" s="31" t="n">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col width="10.83203125" bestFit="1" customWidth="1" style="24" min="2" max="2"/>
+    <col width="15.83203125" bestFit="1" customWidth="1" style="24" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1" s="24">
+      <c r="B1" s="26" t="inlineStr"/>
+    </row>
+    <row r="2" ht="25" customHeight="1" s="24">
+      <c r="B2" s="17" t="n"/>
+      <c r="C2" s="18" t="inlineStr">
+        <is>
+          <t>Unique Counts</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" s="24">
+      <c r="B3" s="19" t="inlineStr">
+        <is>
+          <t>desc1</t>
+        </is>
+      </c>
+      <c r="C3" s="20" t="n">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" s="24">
+      <c r="B4" s="19" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C4" s="20" t="n">
+        <v>13947</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" s="24">
+      <c r="B5" s="19" t="inlineStr">
+        <is>
+          <t>Organization</t>
+        </is>
+      </c>
+      <c r="C5" s="20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" s="24">
+      <c r="B6" s="19" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="C6" s="20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" style="24" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1" s="24">
+      <c r="B1" s="26" t="inlineStr"/>
+    </row>
+    <row r="2" ht="25" customHeight="1" s="24">
+      <c r="B2" s="17" t="n"/>
+      <c r="C2" s="18" t="inlineStr">
+        <is>
+          <t>Date Range</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" s="24">
+      <c r="B3" s="19" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="C3" s="20" t="inlineStr">
+        <is>
+          <t>09/28/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" s="24">
+      <c r="B4" s="19" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="C4" s="20" t="inlineStr">
+        <is>
+          <t>08/25/2023</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" style="24" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1" s="24">
+      <c r="B1" s="27" t="inlineStr">
+        <is>
+          <t>Desc1 Ttesting</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="25" customHeight="1" s="24">
+      <c r="B2" s="28" t="n"/>
+      <c r="C2" s="29" t="inlineStr">
+        <is>
+          <t>P-value</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" s="24">
+      <c r="B3" s="30" t="inlineStr">
+        <is>
+          <t>no_EM</t>
+        </is>
+      </c>
+      <c r="C3" s="32" t="n">
+        <v>0.425231015157453</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" s="24">
+      <c r="B4" s="30" t="inlineStr">
+        <is>
+          <t>no_BK</t>
+        </is>
+      </c>
+      <c r="C4" s="32" t="n">
+        <v>0.04724217184091383</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" s="24">
+      <c r="B5" s="30" t="inlineStr">
+        <is>
+          <t>no_CB</t>
+        </is>
+      </c>
+      <c r="C5" s="32" t="n">
+        <v>2.389479439001783e-11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Further updates on cleaning up code for presentation
</commit_message>
<xml_diff>
--- a/data/visualizations_public.xlsx
+++ b/data/visualizations_public.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lelandmurrin/Data_Science/Capstone_Project_Accounting_Public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2362BA33-71DA-DF44-B0EC-AA426FF314E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A805C32B-D871-B047-8066-01A4CE9009BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-10180" windowWidth="29400" windowHeight="17260" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1860" windowWidth="29400" windowHeight="17260" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lag_stats_CB_172" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,27 @@
     <sheet name="MAPE_Ensemble" sheetId="13" r:id="rId13"/>
     <sheet name="MAPE_Ensemble_Others" sheetId="14" r:id="rId14"/>
     <sheet name="MAPE_ARIMA_Others" sheetId="15" r:id="rId15"/>
+    <sheet name="Summary_Txn_amt" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="166">
   <si>
     <t>Desc1 CB Comparison Table for Periods 4 and 5</t>
   </si>
@@ -294,12 +308,6 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Debit</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
     <t>Txn_amt</t>
   </si>
   <si>
@@ -322,9 +330,6 @@
   </si>
   <si>
     <t>AU 05324</t>
-  </si>
-  <si>
-    <t>--</t>
   </si>
   <si>
     <t>BR</t>
@@ -455,6 +460,9 @@
     <t>Large Transactions by Frequency</t>
   </si>
   <si>
+    <t>Debit</t>
+  </si>
+  <si>
     <t>Freq</t>
   </si>
   <si>
@@ -519,23 +527,79 @@
   </si>
   <si>
     <t>ARIMA Model Results Others</t>
+  </si>
+  <si>
+    <t>Summary of Credit/Debit Transactions</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>75%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -736,7 +800,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1331,11 +1395,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1388,15 +1560,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1442,7 +1608,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1489,6 +1655,34 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1498,12 +1692,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1524,6 +1721,15 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="36" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1837,46 +2043,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
+      <c r="B1" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
     </row>
     <row r="2" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="53"/>
+      <c r="D2" s="61"/>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="52" t="s">
+      <c r="G2" s="61"/>
+      <c r="H2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="52" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="52" t="s">
+      <c r="K2" s="61"/>
+      <c r="L2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="53"/>
+      <c r="M2" s="61"/>
     </row>
     <row r="3" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -2095,128 +2301,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+    </row>
+    <row r="2" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="22">
+        <v>2.3235041965896191E-2</v>
+      </c>
+      <c r="D3" s="22">
+        <v>0.73372243575220197</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="22">
+        <v>-2.4010626649669641E-2</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.75053346663724985</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="22">
+        <v>3.061374543613862E-2</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.67603714017726446</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0.22181641642497621</v>
+      </c>
+      <c r="D6" s="22">
+        <v>4.3454765200988919E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.23164532616789241</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1.369135849657162E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="22">
+        <v>-0.1056222474011311</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.164231931755288</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="22">
+        <v>0.15234345741177441</v>
+      </c>
+      <c r="D9" s="22">
+        <v>4.6358892470148509E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="22">
+        <v>3.5123575115592477E-2</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0.6505046362766006</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-    </row>
-    <row r="2" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="24">
-        <v>2.3235041965896191E-2</v>
-      </c>
-      <c r="D3" s="24">
-        <v>0.73372243575220197</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="24">
-        <v>-2.4010626649669641E-2</v>
-      </c>
-      <c r="D4" s="24">
-        <v>0.75053346663724985</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="24">
-        <v>3.061374543613862E-2</v>
-      </c>
-      <c r="D5" s="24">
-        <v>0.67603714017726446</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="24">
-        <v>0.22181641642497621</v>
-      </c>
-      <c r="D6" s="24">
-        <v>4.3454765200988919E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="24">
-        <v>0.23164532616789241</v>
-      </c>
-      <c r="D7" s="24">
-        <v>1.369135849657162E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="24">
-        <v>-0.1056222474011311</v>
-      </c>
-      <c r="D8" s="24">
-        <v>0.164231931755288</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="23" t="s">
+      <c r="C11" s="22">
+        <v>-9.8811963996663532E-2</v>
+      </c>
+      <c r="D11" s="22">
+        <v>0.20226680376754319</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="24">
-        <v>0.15234345741177441</v>
-      </c>
-      <c r="D9" s="24">
-        <v>4.6358892470148509E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="24">
-        <v>3.5123575115592477E-2</v>
-      </c>
-      <c r="D10" s="24">
-        <v>0.6505046362766006</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="24">
-        <v>-9.8811963996663532E-2</v>
-      </c>
-      <c r="D11" s="24">
-        <v>0.20226680376754319</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="24">
+      <c r="C12" s="22">
         <v>0.25407444787154981</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="22">
         <v>1.565001788636114E-3</v>
       </c>
     </row>
@@ -2243,96 +2449,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="63"/>
+    </row>
+    <row r="2" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="34">
+        <v>83359.94</v>
+      </c>
+      <c r="C3" s="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="55"/>
-    </row>
-    <row r="2" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="36">
-        <v>83359.94</v>
-      </c>
-      <c r="C3" s="35">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="35">
+      <c r="C4" s="33">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36">
+      <c r="B5" s="34">
         <v>84193.7</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36">
+      <c r="B6" s="34">
         <v>135659.45000000001</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="33">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="36">
+      <c r="B7" s="34">
         <v>84049.87</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36">
+      <c r="B8" s="34">
         <v>84324.1</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36">
+      <c r="B9" s="34">
         <v>84603.33</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36">
+      <c r="B10" s="34">
         <v>86289.95</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="36">
+      <c r="B11" s="34">
         <v>91054.02</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="36">
+      <c r="B12" s="34">
         <v>97602.97</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="33">
         <v>2</v>
       </c>
     </row>
@@ -2361,174 +2567,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+    </row>
+    <row r="2" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-    </row>
-    <row r="2" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="E2" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="F2" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="G2" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="H2" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="I2" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="J2" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="K2" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="43" t="s">
+    </row>
+    <row r="3" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="42">
+        <v>0</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="D3" s="43">
+        <v>4</v>
+      </c>
+      <c r="E3" s="43">
+        <v>0</v>
+      </c>
+      <c r="F3" s="43">
+        <v>1</v>
+      </c>
+      <c r="G3" s="43">
+        <v>1</v>
+      </c>
+      <c r="H3" s="43">
+        <v>0</v>
+      </c>
+      <c r="I3" s="43">
+        <v>0</v>
+      </c>
+      <c r="J3" s="43">
+        <v>0</v>
+      </c>
+      <c r="K3" s="44">
+        <v>0.61496967714177142</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="42">
+        <v>1</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="44">
-        <v>0</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="45">
+      <c r="D4" s="43">
         <v>4</v>
       </c>
-      <c r="E3" s="45">
-        <v>0</v>
-      </c>
-      <c r="F3" s="45">
+      <c r="E4" s="43">
         <v>1</v>
       </c>
-      <c r="G3" s="45">
+      <c r="F4" s="43">
+        <v>0</v>
+      </c>
+      <c r="G4" s="43">
+        <v>0</v>
+      </c>
+      <c r="H4" s="43">
+        <v>0</v>
+      </c>
+      <c r="I4" s="43">
+        <v>0</v>
+      </c>
+      <c r="J4" s="43">
+        <v>0</v>
+      </c>
+      <c r="K4" s="44">
+        <v>0.21369813728128659</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="42">
+        <v>2</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="43">
+        <v>3</v>
+      </c>
+      <c r="E5" s="43">
+        <v>0</v>
+      </c>
+      <c r="F5" s="43">
         <v>1</v>
       </c>
-      <c r="H3" s="45">
-        <v>0</v>
-      </c>
-      <c r="I3" s="45">
-        <v>0</v>
-      </c>
-      <c r="J3" s="45">
-        <v>0</v>
-      </c>
-      <c r="K3" s="46">
-        <v>0.61496967714177142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="44">
+      <c r="G5" s="43">
         <v>1</v>
       </c>
-      <c r="C4" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="45">
-        <v>4</v>
-      </c>
-      <c r="E4" s="45">
+      <c r="H5" s="43">
+        <v>0</v>
+      </c>
+      <c r="I5" s="43">
+        <v>0</v>
+      </c>
+      <c r="J5" s="43">
+        <v>0</v>
+      </c>
+      <c r="K5" s="44">
+        <v>0.64183775731186044</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="42">
+        <v>3</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="43">
+        <v>3</v>
+      </c>
+      <c r="E6" s="43">
+        <v>0</v>
+      </c>
+      <c r="F6" s="43">
+        <v>0</v>
+      </c>
+      <c r="G6" s="43">
+        <v>0</v>
+      </c>
+      <c r="H6" s="43">
+        <v>0</v>
+      </c>
+      <c r="I6" s="43">
+        <v>0</v>
+      </c>
+      <c r="J6" s="43">
         <v>1</v>
       </c>
-      <c r="F4" s="45">
-        <v>0</v>
-      </c>
-      <c r="G4" s="45">
-        <v>0</v>
-      </c>
-      <c r="H4" s="45">
-        <v>0</v>
-      </c>
-      <c r="I4" s="45">
-        <v>0</v>
-      </c>
-      <c r="J4" s="45">
-        <v>0</v>
-      </c>
-      <c r="K4" s="46">
-        <v>0.21369813728128659</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="44">
-        <v>2</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="45">
-        <v>3</v>
-      </c>
-      <c r="E5" s="45">
-        <v>0</v>
-      </c>
-      <c r="F5" s="45">
-        <v>1</v>
-      </c>
-      <c r="G5" s="45">
-        <v>1</v>
-      </c>
-      <c r="H5" s="45">
-        <v>0</v>
-      </c>
-      <c r="I5" s="45">
-        <v>0</v>
-      </c>
-      <c r="J5" s="45">
-        <v>0</v>
-      </c>
-      <c r="K5" s="46">
-        <v>0.64183775731186044</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="44">
-        <v>3</v>
-      </c>
-      <c r="C6" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="45">
-        <v>3</v>
-      </c>
-      <c r="E6" s="45">
-        <v>0</v>
-      </c>
-      <c r="F6" s="45">
-        <v>0</v>
-      </c>
-      <c r="G6" s="45">
-        <v>0</v>
-      </c>
-      <c r="H6" s="45">
-        <v>0</v>
-      </c>
-      <c r="I6" s="45">
-        <v>0</v>
-      </c>
-      <c r="J6" s="45">
-        <v>1</v>
-      </c>
-      <c r="K6" s="46">
+      <c r="K6" s="44">
         <v>0.1781559376663141</v>
       </c>
     </row>
@@ -2556,78 +2762,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+    </row>
+    <row r="2" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="35"/>
+      <c r="C2" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="37">
+        <v>0</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-    </row>
-    <row r="2" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="38" t="s">
+      <c r="D3" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="39">
-        <v>0</v>
-      </c>
-      <c r="C3" s="40" t="s">
+      <c r="E3" s="39">
+        <v>0.19077767395010881</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="37">
+        <v>1</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="E4" s="39">
+        <v>0.19122240005791241</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="37">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="41">
-        <v>0.19077767395010881</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="39">
-        <v>1</v>
-      </c>
-      <c r="C4" s="40" t="s">
+      <c r="D5" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="39">
+        <v>0.81587740225031424</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="37">
+        <v>3</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="41">
-        <v>0.19122240005791241</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="39">
-        <v>2</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="41">
-        <v>0.81587740225031424</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="39">
-        <v>3</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>0.73960175688119334</v>
       </c>
     </row>
@@ -2643,7 +2849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -2655,78 +2861,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="64" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="B1" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="48" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="47">
+        <v>0</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="49">
-        <v>0</v>
-      </c>
-      <c r="C3" s="50" t="s">
+      <c r="E3" s="49">
+        <v>0.3707348443913232</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="47">
+        <v>1</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="E4" s="49">
+        <v>0.34070541055434389</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="47">
+        <v>2</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="51">
-        <v>0.3707348443913232</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="49">
-        <v>1</v>
-      </c>
-      <c r="C4" s="50" t="s">
+      <c r="D5" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="49">
+        <v>0.33356490637033559</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="47">
+        <v>3</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="51">
-        <v>0.34070541055434389</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="49">
-        <v>2</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="51">
-        <v>0.33356490637033559</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="49">
-        <v>3</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="51">
+      <c r="E6" s="49">
         <v>0.31002531717376391</v>
       </c>
     </row>
@@ -2755,174 +2961,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
+      <c r="B1" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="F2" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="G2" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="H2" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="I2" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="J2" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="K2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="48" t="s">
+    </row>
+    <row r="3" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="47">
+        <v>0</v>
+      </c>
+      <c r="C3" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="D3" s="48">
+        <v>4</v>
+      </c>
+      <c r="E3" s="48">
+        <v>0</v>
+      </c>
+      <c r="F3" s="48">
+        <v>1</v>
+      </c>
+      <c r="G3" s="48">
+        <v>2</v>
+      </c>
+      <c r="H3" s="48">
+        <v>0</v>
+      </c>
+      <c r="I3" s="48">
+        <v>0</v>
+      </c>
+      <c r="J3" s="48">
+        <v>0</v>
+      </c>
+      <c r="K3" s="49">
+        <v>0.25925601981073498</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="47">
+        <v>1</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="49">
-        <v>0</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="50">
+      <c r="D4" s="48">
         <v>4</v>
       </c>
-      <c r="E3" s="50">
-        <v>0</v>
-      </c>
-      <c r="F3" s="50">
+      <c r="E4" s="48">
         <v>1</v>
       </c>
-      <c r="G3" s="50">
+      <c r="F4" s="48">
+        <v>0</v>
+      </c>
+      <c r="G4" s="48">
+        <v>0</v>
+      </c>
+      <c r="H4" s="48">
+        <v>0</v>
+      </c>
+      <c r="I4" s="48">
+        <v>0</v>
+      </c>
+      <c r="J4" s="48">
+        <v>0</v>
+      </c>
+      <c r="K4" s="49">
+        <v>0.36492051416959442</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="47">
         <v>2</v>
       </c>
-      <c r="H3" s="50">
-        <v>0</v>
-      </c>
-      <c r="I3" s="50">
-        <v>0</v>
-      </c>
-      <c r="J3" s="50">
-        <v>0</v>
-      </c>
-      <c r="K3" s="51">
-        <v>0.25925601981073498</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="49">
+      <c r="C5" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="48">
+        <v>3</v>
+      </c>
+      <c r="E5" s="48">
+        <v>2</v>
+      </c>
+      <c r="F5" s="48">
+        <v>2</v>
+      </c>
+      <c r="G5" s="48">
         <v>1</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="50">
-        <v>4</v>
-      </c>
-      <c r="E4" s="50">
+      <c r="H5" s="48">
+        <v>0</v>
+      </c>
+      <c r="I5" s="48">
+        <v>0</v>
+      </c>
+      <c r="J5" s="48">
+        <v>0</v>
+      </c>
+      <c r="K5" s="49">
+        <v>0.36228805125852293</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="47">
+        <v>3</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="48">
+        <v>3</v>
+      </c>
+      <c r="E6" s="48">
+        <v>0</v>
+      </c>
+      <c r="F6" s="48">
+        <v>0</v>
+      </c>
+      <c r="G6" s="48">
+        <v>0</v>
+      </c>
+      <c r="H6" s="48">
+        <v>0</v>
+      </c>
+      <c r="I6" s="48">
+        <v>0</v>
+      </c>
+      <c r="J6" s="48">
         <v>1</v>
       </c>
-      <c r="F4" s="50">
-        <v>0</v>
-      </c>
-      <c r="G4" s="50">
-        <v>0</v>
-      </c>
-      <c r="H4" s="50">
-        <v>0</v>
-      </c>
-      <c r="I4" s="50">
-        <v>0</v>
-      </c>
-      <c r="J4" s="50">
-        <v>0</v>
-      </c>
-      <c r="K4" s="51">
-        <v>0.36492051416959442</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="49">
-        <v>2</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="50">
-        <v>3</v>
-      </c>
-      <c r="E5" s="50">
-        <v>2</v>
-      </c>
-      <c r="F5" s="50">
-        <v>2</v>
-      </c>
-      <c r="G5" s="50">
-        <v>1</v>
-      </c>
-      <c r="H5" s="50">
-        <v>0</v>
-      </c>
-      <c r="I5" s="50">
-        <v>0</v>
-      </c>
-      <c r="J5" s="50">
-        <v>0</v>
-      </c>
-      <c r="K5" s="51">
-        <v>0.36228805125852293</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="49">
-        <v>3</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="50">
-        <v>3</v>
-      </c>
-      <c r="E6" s="50">
-        <v>0</v>
-      </c>
-      <c r="F6" s="50">
-        <v>0</v>
-      </c>
-      <c r="G6" s="50">
-        <v>0</v>
-      </c>
-      <c r="H6" s="50">
-        <v>0</v>
-      </c>
-      <c r="I6" s="50">
-        <v>0</v>
-      </c>
-      <c r="J6" s="50">
-        <v>1</v>
-      </c>
-      <c r="K6" s="51">
+      <c r="K6" s="49">
         <v>0.33507386955658403</v>
       </c>
     </row>
@@ -2931,6 +3137,133 @@
     <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="B1:D10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+    </row>
+    <row r="2" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="53">
+        <v>3160</v>
+      </c>
+      <c r="D3" s="53">
+        <v>73564</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="53">
+        <v>-380.99335443037972</v>
+      </c>
+      <c r="D4" s="53">
+        <v>1688.1570295253109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="53">
+        <v>3100.5364682198879</v>
+      </c>
+      <c r="D5" s="53">
+        <v>6743.9474029910498</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="53">
+        <v>-142779.98000000001</v>
+      </c>
+      <c r="D6" s="53">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="53">
+        <v>-181.77</v>
+      </c>
+      <c r="D7" s="53">
+        <v>56.64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="53">
+        <v>-67.454999999999998</v>
+      </c>
+      <c r="D8" s="53">
+        <v>127.43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="53">
+        <v>-31.987500000000001</v>
+      </c>
+      <c r="D9" s="53">
+        <v>534.28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="53">
+        <v>-0.02</v>
+      </c>
+      <c r="D10" s="53">
+        <v>193001.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2946,15 +3279,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="2:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="7"/>
@@ -3068,14 +3401,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
@@ -3307,298 +3640,264 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:O7"/>
+  <dimension ref="B1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="15" width="14" customWidth="1"/>
+    <col min="3" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="54" customWidth="1"/>
+    <col min="9" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="56" t="s">
+    <row r="1" spans="2:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-    </row>
-    <row r="2" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="15"/>
-      <c r="C2" s="16" t="s">
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+    </row>
+    <row r="2" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="55"/>
+      <c r="C2" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="N2" s="16" t="s">
+    </row>
+    <row r="3" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="57">
+        <v>28727</v>
+      </c>
+      <c r="C3" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="D3" s="58">
+        <v>5324</v>
+      </c>
+      <c r="E3" s="58" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="17">
-        <v>28727</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="F3" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="59">
+        <v>74.91</v>
+      </c>
+      <c r="H3" s="76">
+        <v>44354</v>
+      </c>
+      <c r="I3" s="58">
+        <v>2021</v>
+      </c>
+      <c r="J3" s="58">
+        <v>9</v>
+      </c>
+      <c r="K3" s="58">
+        <v>20</v>
+      </c>
+      <c r="L3" s="58">
+        <v>23</v>
+      </c>
+      <c r="M3" s="58">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="57">
+        <v>53577</v>
+      </c>
+      <c r="C4" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="18">
-        <v>5324</v>
-      </c>
-      <c r="E3" s="18" t="s">
+      <c r="D4" s="58">
+        <v>9866</v>
+      </c>
+      <c r="E4" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F4" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="19">
-        <v>-74.91</v>
-      </c>
-      <c r="H3" s="18" t="s">
+      <c r="G4" s="59">
+        <v>79.62</v>
+      </c>
+      <c r="H4" s="76">
+        <v>44729</v>
+      </c>
+      <c r="I4" s="58">
+        <v>2022</v>
+      </c>
+      <c r="J4" s="58">
+        <v>9</v>
+      </c>
+      <c r="K4" s="58">
+        <v>32</v>
+      </c>
+      <c r="L4" s="58">
+        <v>24</v>
+      </c>
+      <c r="M4" s="58">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="57">
+        <v>36992</v>
+      </c>
+      <c r="C5" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="19">
-        <v>74.91</v>
-      </c>
-      <c r="J3" s="20">
-        <v>44354</v>
-      </c>
-      <c r="K3" s="18">
+      <c r="D5" s="58">
+        <v>6521</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="59">
+        <v>55.55</v>
+      </c>
+      <c r="H5" s="76">
+        <v>44460</v>
+      </c>
+      <c r="I5" s="58">
         <v>2021</v>
       </c>
-      <c r="L3" s="18">
+      <c r="J5" s="58">
+        <v>12</v>
+      </c>
+      <c r="K5" s="58">
+        <v>23</v>
+      </c>
+      <c r="L5" s="58">
+        <v>38</v>
+      </c>
+      <c r="M5" s="58">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="57">
+        <v>33942</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="58">
+        <v>6040</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="59">
+        <v>475.62</v>
+      </c>
+      <c r="H6" s="76">
+        <v>44417</v>
+      </c>
+      <c r="I6" s="58">
+        <v>2021</v>
+      </c>
+      <c r="J6" s="58">
+        <v>11</v>
+      </c>
+      <c r="K6" s="58">
+        <v>22</v>
+      </c>
+      <c r="L6" s="58">
+        <v>32</v>
+      </c>
+      <c r="M6" s="58">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="57">
+        <v>53920</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="58">
+        <v>9940</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="59">
+        <v>395.67</v>
+      </c>
+      <c r="H7" s="76">
+        <v>44740</v>
+      </c>
+      <c r="I7" s="58">
+        <v>2022</v>
+      </c>
+      <c r="J7" s="58">
         <v>9</v>
       </c>
-      <c r="M3" s="18">
-        <v>20</v>
-      </c>
-      <c r="N3" s="18">
-        <v>23</v>
-      </c>
-      <c r="O3" s="18">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="17">
-        <v>53577</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="18">
-        <v>9866</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="19">
-        <v>-79.62</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I4" s="19">
-        <v>79.62</v>
-      </c>
-      <c r="J4" s="20">
-        <v>44729</v>
-      </c>
-      <c r="K4" s="18">
-        <v>2022</v>
-      </c>
-      <c r="L4" s="18">
-        <v>9</v>
-      </c>
-      <c r="M4" s="18">
+      <c r="K7" s="58">
         <v>32</v>
       </c>
-      <c r="N4" s="18">
-        <v>24</v>
-      </c>
-      <c r="O4" s="18">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="17">
-        <v>36992</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="18">
-        <v>6521</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="19">
-        <v>-55.55</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I5" s="19">
-        <v>55.55</v>
-      </c>
-      <c r="J5" s="20">
-        <v>44460</v>
-      </c>
-      <c r="K5" s="18">
-        <v>2021</v>
-      </c>
-      <c r="L5" s="18">
-        <v>12</v>
-      </c>
-      <c r="M5" s="18">
-        <v>23</v>
-      </c>
-      <c r="N5" s="18">
-        <v>38</v>
-      </c>
-      <c r="O5" s="18">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="17">
-        <v>33942</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="18">
-        <v>6040</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="19">
-        <v>-475.62</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I6" s="19">
-        <v>475.62</v>
-      </c>
-      <c r="J6" s="20">
-        <v>44417</v>
-      </c>
-      <c r="K6" s="18">
-        <v>2021</v>
-      </c>
-      <c r="L6" s="18">
-        <v>11</v>
-      </c>
-      <c r="M6" s="18">
-        <v>22</v>
-      </c>
-      <c r="N6" s="18">
-        <v>32</v>
-      </c>
-      <c r="O6" s="18">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="17">
-        <v>53920</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="18">
-        <v>9940</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="19">
-        <v>-395.67</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I7" s="19">
-        <v>395.67</v>
-      </c>
-      <c r="J7" s="20">
-        <v>44740</v>
-      </c>
-      <c r="K7" s="18">
-        <v>2022</v>
-      </c>
-      <c r="L7" s="18">
-        <v>9</v>
-      </c>
-      <c r="M7" s="18">
-        <v>32</v>
-      </c>
-      <c r="N7" s="18">
+      <c r="L7" s="58">
         <v>26</v>
       </c>
-      <c r="O7" s="18">
+      <c r="M7" s="58">
         <v>144</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3609,7 +3908,7 @@
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3619,18 +3918,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="57"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C3" s="14">
         <v>355</v>
@@ -3646,7 +3945,7 @@
     </row>
     <row r="5" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C5" s="14">
         <v>4</v>
@@ -3682,29 +3981,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="57"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3729,38 +4028,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="55"/>
+      <c r="B1" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="15"/>
       <c r="C2" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="19">
+        <v>114</v>
+      </c>
+      <c r="C3" s="18">
         <v>0.42523101515745299</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="19">
+        <v>115</v>
+      </c>
+      <c r="C4" s="18">
         <v>4.7242171840913831E-2</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="19">
+        <v>116</v>
+      </c>
+      <c r="C5" s="18">
         <v>2.3894794390017829E-11</v>
       </c>
     </row>
@@ -3786,38 +4085,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="63"/>
+    </row>
+    <row r="2" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="30">
+        <v>2.8530607940061539E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="30">
+        <v>6.1547009268820004E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="55"/>
-    </row>
-    <row r="2" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="29"/>
-      <c r="C2" s="30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="32">
-        <v>2.8530607940061539E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="32">
-        <v>6.1547009268820004E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="32">
+      <c r="C5" s="30">
         <v>1.7467156215665861E-8</v>
       </c>
     </row>
@@ -3844,84 +4143,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+    </row>
+    <row r="2" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="23"/>
+      <c r="C2" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-    </row>
-    <row r="2" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="25"/>
-      <c r="C2" s="26" t="s">
+      <c r="C3" s="26">
+        <v>4.0079423901679158E-2</v>
+      </c>
+      <c r="D3" s="26">
+        <v>0.76608565892424929</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="C4" s="26">
+        <v>-0.68261251647126298</v>
+      </c>
+      <c r="D4" s="26">
+        <v>3.3881743663767788E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="25" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
+      <c r="C5" s="26">
+        <v>-9.8774743092295281E-2</v>
+      </c>
+      <c r="D5" s="26">
+        <v>0.59946929399110283</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="28">
-        <v>4.0079423901679158E-2</v>
-      </c>
-      <c r="D3" s="28">
-        <v>0.76608565892424929</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+      <c r="C6" s="26">
+        <v>-7.525903216987942E-2</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0.62990923113574593</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="28">
-        <v>-0.68261251647126298</v>
-      </c>
-      <c r="D4" s="28">
-        <v>3.3881743663767788E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+      <c r="C7" s="26">
+        <v>7.4356806990677579E-2</v>
+      </c>
+      <c r="D7" s="26">
+        <v>0.62053206461626609</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="28">
-        <v>-9.8774743092295281E-2</v>
-      </c>
-      <c r="D5" s="28">
-        <v>0.59946929399110283</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="28">
-        <v>-7.525903216987942E-2</v>
-      </c>
-      <c r="D6" s="28">
-        <v>0.62990923113574593</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="28">
-        <v>7.4356806990677579E-2</v>
-      </c>
-      <c r="D7" s="28">
-        <v>0.62053206461626609</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="28">
+      <c r="C8" s="26">
         <v>-6.0210329575816478E-2</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="26">
         <v>0.70205107936220812</v>
       </c>
     </row>

</xml_diff>